<commit_message>
add continent code in country import
</commit_message>
<xml_diff>
--- a/public/assets/excel/sample_countries.xlsx
+++ b/public/assets/excel/sample_countries.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">continent_id</t>
+    <t xml:space="preserve">continent_code</t>
   </si>
   <si>
     <t xml:space="preserve">name_ar</t>
@@ -116,16 +116,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -321,10 +317,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -359,14 +355,9 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
@@ -378,12 +369,6 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>